<commit_message>
added setBlank(), updated readme
</commit_message>
<xml_diff>
--- a/Methods.xlsx
+++ b/Methods.xlsx
@@ -24,127 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
-  <si>
-    <t>vExcel.vWorksheet PushNewSheet(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet PopSheetByName(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet GetSheetByName(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet RenameSheetByName(System.String, System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet CopySheetByName(System.String, System.String)</t>
-  </si>
-  <si>
-    <t>Void SaveOverride(System.String)</t>
-  </si>
-  <si>
-    <t>Void Close()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SelectCells(Int32, Int32, Int32, Int32)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SelectCell(Int32, Int32)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetValue(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet ReplaceValue(System.String, System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet ReplaceValueContaining(System.String, System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet ClearValue()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontSize(Int32)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontColor(System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontFamily(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontBold(Boolean)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontItalic(Boolean)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontUnderline(Boolean)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontStrikethrough(Boolean)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontHorizontalCenter()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontHorizontalLeft()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontHorizontalRight()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontVerticalCenter()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontVerticalBottom()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetFontVerticalTop()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet AutoSizeColumns()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet AutoSizeColumnsRelative()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderWeights(Double, Double, Double, Double)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderWeightsEach(Double, Double, Double, Double)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderWeightEach(Double)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderBottom(Double, System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderWeight(Double)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderColors(System.Drawing.Color, System.Drawing.Color, System.Drawing.Color, System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderColorsEach(System.Drawing.Color, System.Drawing.Color, System.Drawing.Color, System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderColorEach(System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetDefaultBorder()</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBorderColor(System.Drawing.Color)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetComment(System.String)</t>
-  </si>
-  <si>
-    <t>vExcel.vWorksheet SetBackgroundColor(System.Drawing.Color)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>Copies and returns the copy sheet</t>
   </si>
@@ -167,9 +47,6 @@
     <t>Coordinate of top-left and bottom-right cell</t>
   </si>
   <si>
-    <t>Replace values from matching substring</t>
-  </si>
-  <si>
     <t>Autosize entire column based on the current selected cell.</t>
   </si>
   <si>
@@ -177,6 +54,141 @@
   </si>
   <si>
     <t>Applies per cell</t>
+  </si>
+  <si>
+    <t>PushNewSheet(String Name)</t>
+  </si>
+  <si>
+    <t>PopSheetByName(String TabLabel)</t>
+  </si>
+  <si>
+    <t>GetSheetByName(String TabLabel)</t>
+  </si>
+  <si>
+    <t>RenameSheetByName(String current, String newName)</t>
+  </si>
+  <si>
+    <t>CopySheetByName(String current, String newName)</t>
+  </si>
+  <si>
+    <t>SaveOverride(String path)</t>
+  </si>
+  <si>
+    <t>Close()</t>
+  </si>
+  <si>
+    <t>SelectCells(Int32 TopX, Int32 TopY, Int32 BottomX, Int32 BottomY)</t>
+  </si>
+  <si>
+    <t>SelectCell(Int32 X, Int32 Y)</t>
+  </si>
+  <si>
+    <t>SetValue(String value)</t>
+  </si>
+  <si>
+    <t>ReplaceValue(String current, String newValue)</t>
+  </si>
+  <si>
+    <t>ReplaceValueContaining(String containValue, String newValue)</t>
+  </si>
+  <si>
+    <t>ClearValue()</t>
+  </si>
+  <si>
+    <t>SetFontSize(Int32 size)</t>
+  </si>
+  <si>
+    <t>SetFontColor(Color Color)</t>
+  </si>
+  <si>
+    <t>SetFontFamily(String family)</t>
+  </si>
+  <si>
+    <t>SetFontBold(Boolean isBold)</t>
+  </si>
+  <si>
+    <t>SetFontItalic(Boolean isItalic)</t>
+  </si>
+  <si>
+    <t>SetFontUnderline(Boolean isUnderline)</t>
+  </si>
+  <si>
+    <t>SetFontStrikethrough(Boolean isStrikethrough)</t>
+  </si>
+  <si>
+    <t>SetFontHorizontalCenter()</t>
+  </si>
+  <si>
+    <t>SetFontHorizontalLeft()</t>
+  </si>
+  <si>
+    <t>SetFontHorizontalRight()</t>
+  </si>
+  <si>
+    <t>SetFontVerticalCenter()</t>
+  </si>
+  <si>
+    <t>SetFontVerticalBottom()</t>
+  </si>
+  <si>
+    <t>SetFontVerticalTop()</t>
+  </si>
+  <si>
+    <t>AutoSizeColumns()</t>
+  </si>
+  <si>
+    <t>AutoSizeColumnsRelative()</t>
+  </si>
+  <si>
+    <t>SetBorderWeights(Double Top, Double Right, Double Bottom, Double Left)</t>
+  </si>
+  <si>
+    <t>SetBorderWeightsEach(Double Top, Double Right, Double Bottom, Double Left)</t>
+  </si>
+  <si>
+    <t>SetBorderWeightEach(Double weight)</t>
+  </si>
+  <si>
+    <t>SetBorderBottom(Double Weight, Color Color)</t>
+  </si>
+  <si>
+    <t>SetBorderWeight(Double thickness)</t>
+  </si>
+  <si>
+    <t>SetBorderColors(Color Top, Color Right, Color Bottom, Color Left)</t>
+  </si>
+  <si>
+    <t>SetBorderColorsEach(Color Top, Color Right, Color Bottom, Color Left)</t>
+  </si>
+  <si>
+    <t>SetBorderColorEach(Color Color)</t>
+  </si>
+  <si>
+    <t>SetDefaultBorder()</t>
+  </si>
+  <si>
+    <t>SetBlank()</t>
+  </si>
+  <si>
+    <t>SetBorderColor(Color Color)</t>
+  </si>
+  <si>
+    <t>SetComment(String comment)</t>
+  </si>
+  <si>
+    <t>RemoveComment()</t>
+  </si>
+  <si>
+    <t>SetBackgroundColor(Color color)</t>
+  </si>
+  <si>
+    <t>Replace value if entire string is matched</t>
+  </si>
+  <si>
+    <t>Replace value from matching substring</t>
+  </si>
+  <si>
+    <t>Set background to default color and removes any presence of borders. Font is not affected.</t>
   </si>
 </sst>
 </file>
@@ -494,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B43"/>
+  <dimension ref="A2:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,322 +520,338 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>